<commit_message>
Spring security helloworld: documentation
</commit_message>
<xml_diff>
--- a/spring-security-helloworld-xml/Readme/spring-security-helloworld-xml.xlsx
+++ b/spring-security-helloworld-xml/Readme/spring-security-helloworld-xml.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E405A3F-275C-4E6E-A58F-E3741875BB76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72998271-7B43-4EFD-AA4B-E2D52B6C7A46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pom" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="178">
   <si>
     <t>properties</t>
   </si>
@@ -1383,7 +1383,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>import org.springframework.stereotype.Controller;</t>
+      <t>import org.springframework.web.bind.annotation.RequestMapping;</t>
     </r>
     <r>
       <rPr>
@@ -1395,6 +1395,285 @@
       </rPr>
       <t xml:space="preserve">
 import ...
+@Controller
+public class HelloController {
+   @RequestMapping(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value = { "/", "/welcome**" }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, method = RequestMethod.GET)
+   public ModelAndView welcomePage() {
+      ...
+   }
+   ...
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/bind/annotation/RequestMapping.html#value--</t>
+  </si>
+  <si>
+    <t>String[], RequestMapping</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>RequestMethod</t>
+  </si>
+  <si>
+    <t>public abstract RequestMethod[] method
+The HTTP request methods to map to, narrowing the primary mapping: GET, POST, HEAD, OPTIONS, PUT, PATCH, DELETE, TRACE.
+Supported at the type level as well as at the method level! When used at the type level, all method-level mappings inherit this HTTP method restriction (i.e. the type-level restriction gets checked before the handler method is even resolved).
+Default:
+{}</t>
+  </si>
+  <si>
+    <t>"@AliasFor(value="path")"
+public abstract String[] value
+The primary mapping expressed by this annotation.
+This is an alias for path(). For example @RequestMapping("/foo") is equivalent to @RequestMapping(path="/foo").
+Supported at the type level as well as at the method level! When used at the type level, all method-level mappings inherit this primary mapping, narrowing it for a specific handler method.
+Default:
+{}</t>
+  </si>
+  <si>
+    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/bind/annotation/RequestMapping.html#method--</t>
+  </si>
+  <si>
+    <t>Enum Constant</t>
+  </si>
+  <si>
+    <t>public enum RequestMethod
+extends Enum&lt;RequestMethod&gt;
+Java 5 enumeration of HTTP request methods. Intended for use with the RequestMapping.method() attribute of the RequestMapping annotation.
+Note that, by default, DispatcherServlet supports GET, HEAD, POST, PUT, PATCH and DELETE only. DispatcherServlet will process TRACE and OPTIONS with the default HttpServlet behavior unless explicitly told to dispatch those request types as well: Check out the "dispatchOptionsRequest" and "dispatchTraceRequest" properties, switching them to "true" if necessary.</t>
+  </si>
+  <si>
+    <r>
+      <t>import org.springframework.web.bind.annotation.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RequestMethod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+...
+@Controller
+public class HelloController {
+   @RequestMapping(value = { "/", "/welcome**" }, method = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RequestMethod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.GET)
+   public ModelAndView welcomePage() {
+      ...
+   }
+   ...
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>import org.springframework.web.bind.annotation.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RequestMapping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+import ...
+@Controller
+public class HelloController {
+   @RequestMapping(value = { "/", "/welcome**" }, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>method = RequestMethod.GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+   public ModelAndView welcomePage() {
+      ...
+   }
+   ...
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>import org.springframework.web.bind.annotation.RequestMapping;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+...
+@Controller
+public class HelloController {
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@RequestMapping(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value = { "/", "/welcome**" }, method = RequestMethod.GET</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   public ModelAndView welcomePage() {
+      ...
+   }
+   ...
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>import org.springframework.stereotype.Controller;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+...
 </t>
     </r>
     <r>
@@ -1436,7 +1715,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>import org.springframework.web.bind.annotation.RequestMapping;</t>
+      <t>import org.springframework.web.servlet.ModelAndView;</t>
     </r>
     <r>
       <rPr>
@@ -1447,42 +1726,278 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-import ...
-@Controller
+…
 public class HelloController {
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@RequestMapping(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>value = { "/", "/welcome**" }, method = RequestMethod.GET</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
+   ...
+   public </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ModelAndView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> welcomePage() {
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ModelAndView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ModelAndView()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.addObject("title", "Spring Security Hello World");
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.addObject("message", "This is welcome page!");
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.setViewName("hello");
+      return </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+   }
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/servlet/ModelAndView.html</t>
+  </si>
+  <si>
+    <t>ModelAndView</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>public class ModelAndView
+extends Object
+Holder for both Model and View in the web MVC framework. Note that these are entirely distinct. This class merely holds both to make it possible for a controller to return both model and view in a single return value.
+Represents a model and view returned by a handler, to be resolved by a DispatcherServlet. The view can take the form of a String view name which will need to be resolved by a ViewResolver object; alternatively a View object can be specified directly. The model is a Map, allowing the use of multiple objects keyed by name.</t>
+  </si>
+  <si>
+    <t>addObject</t>
+  </si>
+  <si>
+    <t>public ModelAndView addObject(String attributeName,
+                              @Nullable
+                              Object attributeValue)
+Add an attribute to the model.
+Parameters:
+attributeName - name of the object to add to the model (never null)
+attributeValue - object to add to the model (can be null)</t>
+  </si>
+  <si>
+    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/servlet/ModelAndView.html#addObject-java.lang.String-java.lang.Object-</t>
+  </si>
+  <si>
+    <t>setView</t>
+  </si>
+  <si>
+    <t>public void setView(@Nullable
+                    View view)
+Set a View object for this ModelAndView. Will override any pre-existing view name or View.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>import org.springframework.web.servlet.ModelAndView;</t>
     </r>
     <r>
       <rPr>
@@ -1493,173 +2008,113 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+…
+public class HelloController {
+   ...
    public ModelAndView welcomePage() {
-      ...
+      ModelAndView model = new ModelAndView();
+      model.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>addObject("title", "Spring Security Hello World")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+      model.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>addObject("message", "This is welcome page!")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+      model.setViewName("hello");
+      return model;
    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>import org.springframework.web.servlet.ModelAndView;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+…
+public class HelloController {
    ...
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>import org.springframework.web.bind.annotation.RequestMapping;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-import ...
-@Controller
-public class HelloController {
-   @RequestMapping(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>value = { "/", "/welcome**" }</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, method = RequestMethod.GET)
    public ModelAndView welcomePage() {
-      ...
+      ModelAndView model = new ModelAndView();
+      model.addObject("title", "Spring Security Hello World");
+      model.addObject("message", "This is welcome page!");
+      model.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setViewName("hello")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+      return model;
    }
-   ...
-}</t>
-    </r>
-  </si>
-  <si>
-    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/bind/annotation/RequestMapping.html#value--</t>
-  </si>
-  <si>
-    <t>String[], RequestMapping</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>RequestMethod</t>
-  </si>
-  <si>
-    <t>public abstract RequestMethod[] method
-The HTTP request methods to map to, narrowing the primary mapping: GET, POST, HEAD, OPTIONS, PUT, PATCH, DELETE, TRACE.
-Supported at the type level as well as at the method level! When used at the type level, all method-level mappings inherit this HTTP method restriction (i.e. the type-level restriction gets checked before the handler method is even resolved).
-Default:
-{}</t>
-  </si>
-  <si>
-    <t>"@AliasFor(value="path")"
-public abstract String[] value
-The primary mapping expressed by this annotation.
-This is an alias for path(). For example @RequestMapping("/foo") is equivalent to @RequestMapping(path="/foo").
-Supported at the type level as well as at the method level! When used at the type level, all method-level mappings inherit this primary mapping, narrowing it for a specific handler method.
-Default:
-{}</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">import org.springframework.web.bind.annotation.RequestMapping;
-import ...
-@Controller
-public class HelloController {
-   @RequestMapping(value = { "/", "/welcome**" }, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>method = RequestMethod.GET</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-   public ModelAndView welcomePage() {
-      ...
-   }
-   ...
-}</t>
-    </r>
-  </si>
-  <si>
-    <t>https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/bind/annotation/RequestMapping.html#method--</t>
-  </si>
-  <si>
-    <t>Enum Constant</t>
-  </si>
-  <si>
-    <t>public enum RequestMethod
-extends Enum&lt;RequestMethod&gt;
-Java 5 enumeration of HTTP request methods. Intended for use with the RequestMapping.method() attribute of the RequestMapping annotation.
-Note that, by default, DispatcherServlet supports GET, HEAD, POST, PUT, PATCH and DELETE only. DispatcherServlet will process TRACE and OPTIONS with the default HttpServlet behavior unless explicitly told to dispatch those request types as well: Check out the "dispatchOptionsRequest" and "dispatchTraceRequest" properties, switching them to "true" if necessary.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">import org.springframework.web.bind.annotation.RequestMapping;
-import ...
-@Controller
-public class HelloController {
-   @RequestMapping(value = { "/", "/welcome**" }, method = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RequestMethod</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.GET)
-   public ModelAndView welcomePage() {
-      ...
-   }
-   ...
 }</t>
     </r>
   </si>
@@ -2279,12 +2734,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2411,108 +2863,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2539,15 +2889,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2582,32 +2923,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2621,35 +3055,68 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2948,290 +3415,291 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="141" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="142"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="102"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="74"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="119"/>
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="76"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="115"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="119"/>
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="76"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="115"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81"/>
-      <c r="B6" s="30" t="s">
+      <c r="A6" s="120"/>
+      <c r="B6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="77"/>
-      <c r="E6" s="78"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="117"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="83"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="110"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="82" t="s">
+      <c r="A10" s="110"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="83"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="122"/>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="6" t="s">
+      <c r="A12" s="110"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="33" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="63" t="s">
+      <c r="A13" s="110"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="64"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="106"/>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="6" t="s">
+      <c r="A15" s="110"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="33" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="110"/>
+      <c r="B16" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="83"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="122"/>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="71"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="6" t="s">
+      <c r="A18" s="110"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="63" t="s">
+      <c r="A19" s="110"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="64"/>
+      <c r="A20" s="110"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="106"/>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="6" t="s">
+      <c r="A21" s="110"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="67" t="s">
+      <c r="A22" s="110"/>
+      <c r="B22" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="34" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="64"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="106"/>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="72"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="6" t="s">
+      <c r="A24" s="111"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C13:C15"/>
     <mergeCell ref="B7:B15"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E2"/>
@@ -3248,7 +3716,6 @@
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3260,141 +3727,192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1FE5DB-82D1-4DD7-AB96-2627786C492E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="113.7109375" customWidth="1"/>
     <col min="4" max="4" width="76.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="134.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="133" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="126" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="134"/>
-      <c r="E2" s="135"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="139" t="s">
+      <c r="D3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="140" t="s">
+      <c r="E3" s="93" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
+    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="120" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="255" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E6" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="102" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="126" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="126" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="127" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="130" t="s">
+      <c r="C7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="B8" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" s="127" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="102" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="C8" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="127" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="127" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A10" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="76"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3407,9 +3925,12 @@
     <hyperlink ref="E6" r:id="rId3" location="value--" xr:uid="{351D0148-4479-462D-B0AD-4679C127E526}"/>
     <hyperlink ref="E7" r:id="rId4" location="method--" xr:uid="{28778C99-D61C-4724-863B-77ACBE9B0982}"/>
     <hyperlink ref="E8" r:id="rId5" location="method--" xr:uid="{1F708173-FE61-4515-9FD2-EC9839716367}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{C4F24B64-CF60-4366-97C4-2158956D1E93}"/>
+    <hyperlink ref="E10" r:id="rId7" location="addObject-java.lang.String-java.lang.Object-" xr:uid="{100143C2-61DC-4A9E-B676-BA7500BBC06C}"/>
+    <hyperlink ref="E11" r:id="rId8" location="addObject-java.lang.String-java.lang.Object-" xr:uid="{CAA66A17-50CC-4E3C-A680-9E39C93F1D81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;CAuthor: Boyuan Zhang</oddHeader>
   </headerFooter>
@@ -3434,132 +3955,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="108" t="s">
+      <c r="B1" s="129"/>
+      <c r="C1" s="130" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="108"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="73" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="70" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="62" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="63" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="63" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="99" t="s">
+      <c r="E7" s="64" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="114" t="s">
+      <c r="A8" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="E8" s="101" t="s">
+      <c r="E8" s="66" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3590,287 +4111,287 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" style="19" customWidth="1"/>
-    <col min="4" max="4" width="91.28515625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="73.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="19"/>
-    <col min="9" max="9" width="123" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.85546875" style="19" customWidth="1"/>
-    <col min="12" max="12" width="56.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="19"/>
-    <col min="15" max="15" width="36" style="19" customWidth="1"/>
-    <col min="16" max="16" width="123" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="15.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="91.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="73.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="18"/>
+    <col min="9" max="9" width="123" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="56.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="18"/>
+    <col min="15" max="15" width="36" style="18" customWidth="1"/>
+    <col min="16" max="16" width="123" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="139" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="91" t="s">
+      <c r="B1" s="140"/>
+      <c r="C1" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="56"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="45" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="45" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:18" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="45" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="51"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="92" t="s">
+      <c r="A11" s="60"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="57"/>
+      <c r="D11" s="138"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="136"/>
+      <c r="C12" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="88"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="134"/>
+      <c r="E12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="59" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="85" t="s">
+      <c r="B13" s="136"/>
+      <c r="C13" s="131" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="58" t="s">
+      <c r="D13" s="132"/>
+      <c r="E13" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="21"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="20"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="21"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="20"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="21"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="20"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3903,299 +4424,298 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E47D01-5FB3-4DF7-AF2E-7290FE93ACCF}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.28515625" customWidth="1"/>
-    <col min="5" max="5" width="63.85546875" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="141" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="141" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="141" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.28515625" style="141" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" style="141" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="141" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="95" t="s">
+      <c r="C1" s="143"/>
+      <c r="D1" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="145"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="146" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="147" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="148" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>